<commit_message>
Fix many to 1 schedules
Event facilities that require multiple schedules will not be handled properly. The solution was to split the "Siemens Schedule" values by ',' and duplicate all of the other row information so that the matching apparatus still works properly. This just creates a redundancy under the "Who booked this room" section, but that is not a true issue.

Updated Everson Class Schedule to be "Can not schedule" Updated MU S8 to be inside of the tower group.
</commit_message>
<xml_diff>
--- a/src/AHU inventory.xlsx
+++ b/src/AHU inventory.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="496">
   <si>
     <t>Building</t>
   </si>
@@ -1383,9 +1383,6 @@
     <t>MSC.AH6.SCHEDULE</t>
   </si>
   <si>
-    <t>Rec Hall Main Floor_Schedule, Rec Hall_Schedule</t>
-  </si>
-  <si>
     <t>Young Hall Fan Coil Rooms</t>
   </si>
   <si>
@@ -1404,9 +1401,6 @@
     <t>MU MUII TOWER SCHEDULE</t>
   </si>
   <si>
-    <t>Everson Class Schedule</t>
-  </si>
-  <si>
     <t>ART BLDG SCHEDULE</t>
   </si>
   <si>
@@ -1434,18 +1428,12 @@
     <t>BAINER HALL TOWER AC SCHEDULE</t>
   </si>
   <si>
-    <t>MU S8 SCHEDULE</t>
-  </si>
-  <si>
     <t>RM 2405</t>
   </si>
   <si>
     <t>All AHUs - need to make group in siemens scheduler</t>
   </si>
   <si>
-    <t>SCC.CONFERENCE.ZONE, SCC.BLDG.ZONE</t>
-  </si>
-  <si>
     <t xml:space="preserve">MULTI-PURPOSE ROOM W/ S. </t>
   </si>
   <si>
@@ -1455,24 +1443,12 @@
     <t>Rec Hall Main Floor_Schedule</t>
   </si>
   <si>
-    <t>GSM.AHU2.ZONE, GSM.AHU3.ZONE, GSM.AHU4.ZONE, GSM.CP.SYSTEM.ZONE, GSM.WINDOW.CONF1.ZONE, GSM.WINDOW.CONF2.ZONE</t>
-  </si>
-  <si>
     <t>GSM.AHU2.ZONE</t>
   </si>
   <si>
     <t>GSM.AHU4.ZONE</t>
   </si>
   <si>
-    <t>GSM.AHU3.ZONE, GSM.CP.SYSTEM.ZONE, GSM.WINDOW.CONF1.ZONE, GSM.WINDOW.CONF2.ZONE</t>
-  </si>
-  <si>
-    <t>GSM.AHU2.ZONE, GSM.AHU4.ZONE, GSM.CP.SYSTEM.ZONE, GSM.WINDOW.CONF1.ZONE, GSM.WINDOW.CONF2.ZONE</t>
-  </si>
-  <si>
-    <t>SCC.BLDG.ZONE, SCC.CCC.ZONE</t>
-  </si>
-  <si>
     <t>AC1 probably, need to confirm drawings</t>
   </si>
   <si>
@@ -1536,9 +1512,6 @@
     <t>RM 0165</t>
   </si>
   <si>
-    <t>ARC AHU1 SCHEDULE, ARC AHU2 SCHEDULE</t>
-  </si>
-  <si>
     <t>RM 2406</t>
   </si>
   <si>
@@ -1560,9 +1533,6 @@
     <t>DRAMA AC06 SCHEDULE</t>
   </si>
   <si>
-    <t>DRAMA AC05 SCHEDULE, DRAMA AC06 SCHEDULE, DRAMA AC07 SCHEDULE</t>
-  </si>
-  <si>
     <t>SCHOOL OF ED. E. LAWN</t>
   </si>
   <si>
@@ -1573,6 +1543,33 @@
   </si>
   <si>
     <t>ARC AHU7 SCHEDULE</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>ARC AHU1 SCHEDULE,ARC AHU2 SCHEDULE</t>
+  </si>
+  <si>
+    <t>DRAMA AC05 SCHEDULE,DRAMA AC06 SCHEDULE,DRAMA AC07 SCHEDULE</t>
+  </si>
+  <si>
+    <t>Rec Hall Main Floor_Schedule,Rec Hall_Schedule</t>
+  </si>
+  <si>
+    <t>SCC.BLDG.ZONE,SCC.CCC.ZONE</t>
+  </si>
+  <si>
+    <t>SCC.CONFERENCE.ZONE,SCC.BLDG.ZONE</t>
+  </si>
+  <si>
+    <t>GSM.AHU2.ZONE,GSM.AHU3.ZONE,GSM.AHU4.ZONE,GSM.CP.SYSTEM.ZONE,GSM.WINDOW.CONF1.ZONE,GSM.WINDOW.CONF2.ZONE</t>
+  </si>
+  <si>
+    <t>GSM.AHU2.ZONE,GSM.AHU4.ZONE,GSM.CP.SYSTEM.ZONE,GSM.WINDOW.CONF1.ZONE,GSM.WINDOW.CONF2.ZONE</t>
+  </si>
+  <si>
+    <t>GSM.AHU3.ZONE,GSM.CP.SYSTEM.ZONE,GSM.WINDOW.CONF1.ZONE,GSM.WINDOW.CONF2.ZONE</t>
   </si>
 </sst>
 </file>
@@ -2061,8 +2058,8 @@
   <dimension ref="A1:G340"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
+      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F191" sqref="F191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2075,7 +2072,7 @@
     <col min="6" max="6" width="122.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2094,8 +2091,11 @@
       <c r="F1" s="2" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -2834,10 +2834,10 @@
         <v>404</v>
       </c>
       <c r="F54" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="G54" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2991,10 +2991,10 @@
         <v>404</v>
       </c>
       <c r="F65" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="G65" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3008,10 +3008,10 @@
         <v>404</v>
       </c>
       <c r="F66" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="G66" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3025,10 +3025,10 @@
         <v>404</v>
       </c>
       <c r="F67" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="G67" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3042,10 +3042,10 @@
         <v>404</v>
       </c>
       <c r="F68" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="G68" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3059,10 +3059,10 @@
         <v>404</v>
       </c>
       <c r="F69" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="G69" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3076,10 +3076,10 @@
         <v>404</v>
       </c>
       <c r="F70" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="G70" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3093,10 +3093,10 @@
         <v>404</v>
       </c>
       <c r="F71" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="G71" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3124,10 +3124,10 @@
         <v>404</v>
       </c>
       <c r="F73" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G73" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3141,7 +3141,7 @@
         <v>404</v>
       </c>
       <c r="F74" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3155,10 +3155,10 @@
         <v>404</v>
       </c>
       <c r="F75" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="G75" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -3172,10 +3172,10 @@
         <v>404</v>
       </c>
       <c r="F76" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="G76" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -3189,10 +3189,10 @@
         <v>404</v>
       </c>
       <c r="F77" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="G77" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -3206,7 +3206,7 @@
         <v>404</v>
       </c>
       <c r="F78" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -3220,7 +3220,7 @@
         <v>404</v>
       </c>
       <c r="F79" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -3285,7 +3285,7 @@
         <v>403</v>
       </c>
       <c r="F83" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3302,7 +3302,7 @@
         <v>404</v>
       </c>
       <c r="F84" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3344,10 +3344,10 @@
         <v>404</v>
       </c>
       <c r="F87" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="G87" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3364,7 +3364,7 @@
         <v>419</v>
       </c>
       <c r="G88" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3378,10 +3378,10 @@
         <v>404</v>
       </c>
       <c r="F89" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="G89" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3412,7 +3412,7 @@
         <v>404</v>
       </c>
       <c r="F91" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3665,7 +3665,7 @@
         <v>404</v>
       </c>
       <c r="F108" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -3693,7 +3693,7 @@
         <v>404</v>
       </c>
       <c r="F110" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3777,10 +3777,10 @@
         <v>404</v>
       </c>
       <c r="F116" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G116" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3982,10 +3982,10 @@
         <v>404</v>
       </c>
       <c r="F130" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G130" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4204,7 +4204,7 @@
         <v>419</v>
       </c>
       <c r="G145" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -4218,10 +4218,10 @@
         <v>404</v>
       </c>
       <c r="F146" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="G146" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -4235,7 +4235,7 @@
         <v>404</v>
       </c>
       <c r="F147" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -4249,7 +4249,7 @@
         <v>404</v>
       </c>
       <c r="F148" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G148">
         <v>438</v>
@@ -4266,10 +4266,10 @@
         <v>404</v>
       </c>
       <c r="F149" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="G149" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -4283,7 +4283,7 @@
         <v>404</v>
       </c>
       <c r="F150" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="G150">
         <v>214</v>
@@ -4300,7 +4300,7 @@
         <v>404</v>
       </c>
       <c r="F151" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="G151">
         <v>212</v>
@@ -4990,7 +4990,7 @@
         <v>404</v>
       </c>
       <c r="F193" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -5004,7 +5004,7 @@
         <v>404</v>
       </c>
       <c r="F194" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -5018,7 +5018,7 @@
         <v>404</v>
       </c>
       <c r="F195" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -5032,7 +5032,7 @@
         <v>404</v>
       </c>
       <c r="F196" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>404</v>
       </c>
       <c r="F197" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -5060,7 +5060,7 @@
         <v>404</v>
       </c>
       <c r="F198" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -5074,7 +5074,7 @@
         <v>404</v>
       </c>
       <c r="F199" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -5088,7 +5088,7 @@
         <v>404</v>
       </c>
       <c r="F200" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -5102,7 +5102,7 @@
         <v>404</v>
       </c>
       <c r="F201" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -5116,7 +5116,7 @@
         <v>404</v>
       </c>
       <c r="F202" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -5130,7 +5130,7 @@
         <v>404</v>
       </c>
       <c r="F203" t="s">
-        <v>433</v>
+        <v>490</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -5144,7 +5144,7 @@
         <v>404</v>
       </c>
       <c r="F204" t="s">
-        <v>433</v>
+        <v>490</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -5158,7 +5158,7 @@
         <v>404</v>
       </c>
       <c r="F205" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -5172,7 +5172,7 @@
         <v>404</v>
       </c>
       <c r="F206" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -5285,10 +5285,10 @@
         <v>404</v>
       </c>
       <c r="F213" t="s">
-        <v>462</v>
+        <v>491</v>
       </c>
       <c r="G213" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -5302,10 +5302,10 @@
         <v>404</v>
       </c>
       <c r="F214" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G214" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -5319,7 +5319,7 @@
         <v>404</v>
       </c>
       <c r="F215" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G215" t="s">
         <v>420</v>
@@ -5336,7 +5336,7 @@
         <v>404</v>
       </c>
       <c r="F216" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G216" t="s">
         <v>421</v>
@@ -5353,7 +5353,7 @@
         <v>404</v>
       </c>
       <c r="F217" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G217" t="s">
         <v>422</v>
@@ -5370,7 +5370,7 @@
         <v>404</v>
       </c>
       <c r="F218" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G218" t="s">
         <v>423</v>
@@ -5387,7 +5387,7 @@
         <v>404</v>
       </c>
       <c r="F219" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G219" t="s">
         <v>424</v>
@@ -5398,13 +5398,13 @@
         <v>43</v>
       </c>
       <c r="B220" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="C220" t="s">
         <v>404</v>
       </c>
       <c r="F220" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -5418,7 +5418,7 @@
         <v>404</v>
       </c>
       <c r="F221" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G221" t="s">
         <v>425</v>
@@ -5439,7 +5439,7 @@
         <v>-1</v>
       </c>
       <c r="F222" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G222" t="s">
         <v>426</v>
@@ -5450,13 +5450,13 @@
         <v>43</v>
       </c>
       <c r="B223" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C223" t="s">
         <v>404</v>
       </c>
       <c r="F223" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G223" t="s">
         <v>426</v>
@@ -5473,7 +5473,7 @@
         <v>404</v>
       </c>
       <c r="F224" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G224" t="s">
         <v>427</v>
@@ -5490,10 +5490,10 @@
         <v>404</v>
       </c>
       <c r="F225" t="s">
-        <v>453</v>
+        <v>492</v>
       </c>
       <c r="G225" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -6066,7 +6066,7 @@
         <v>419</v>
       </c>
       <c r="G264" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
@@ -6083,7 +6083,7 @@
         <v>419</v>
       </c>
       <c r="G265" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
@@ -6100,7 +6100,7 @@
         <v>419</v>
       </c>
       <c r="G266" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
@@ -6117,7 +6117,7 @@
         <v>419</v>
       </c>
       <c r="G267" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
@@ -6215,7 +6215,7 @@
         <v>404</v>
       </c>
       <c r="F274" t="s">
-        <v>457</v>
+        <v>493</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
@@ -6229,7 +6229,7 @@
         <v>404</v>
       </c>
       <c r="F275" t="s">
-        <v>461</v>
+        <v>494</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
@@ -6243,7 +6243,7 @@
         <v>404</v>
       </c>
       <c r="F276" t="s">
-        <v>461</v>
+        <v>494</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
@@ -6257,7 +6257,7 @@
         <v>404</v>
       </c>
       <c r="F277" t="s">
-        <v>460</v>
+        <v>495</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
@@ -6271,7 +6271,7 @@
         <v>404</v>
       </c>
       <c r="F278" t="s">
-        <v>460</v>
+        <v>495</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
@@ -6285,7 +6285,7 @@
         <v>404</v>
       </c>
       <c r="F279" t="s">
-        <v>460</v>
+        <v>495</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
@@ -6299,7 +6299,7 @@
         <v>404</v>
       </c>
       <c r="F280" t="s">
-        <v>460</v>
+        <v>495</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
@@ -6313,7 +6313,7 @@
         <v>404</v>
       </c>
       <c r="F281" t="s">
-        <v>460</v>
+        <v>495</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
@@ -6327,7 +6327,7 @@
         <v>404</v>
       </c>
       <c r="F282" t="s">
-        <v>460</v>
+        <v>495</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
@@ -6403,7 +6403,7 @@
         <v>404</v>
       </c>
       <c r="F287" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
@@ -6417,10 +6417,10 @@
         <v>404</v>
       </c>
       <c r="F288" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="G288" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
@@ -6434,7 +6434,7 @@
         <v>404</v>
       </c>
       <c r="F289" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
@@ -7210,7 +7210,7 @@
         <v>419</v>
       </c>
       <c r="G335" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.25">
@@ -7238,7 +7238,7 @@
         <v>404</v>
       </c>
       <c r="F337" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.25">
@@ -7252,7 +7252,7 @@
         <v>404</v>
       </c>
       <c r="F338" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="339" spans="1:6" x14ac:dyDescent="0.25">
@@ -7266,12 +7266,12 @@
         <v>404</v>
       </c>
       <c r="F339" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="F340" t="s">
         <v>419</v>
@@ -7306,7 +7306,7 @@
   <sheetData>
     <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7317,7 +7317,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7328,7 +7328,7 @@
         <v>115</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7339,7 +7339,7 @@
         <v>120</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7350,7 +7350,7 @@
         <v>151</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7361,7 +7361,7 @@
         <v>204</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7372,7 +7372,7 @@
         <v>211</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7383,7 +7383,7 @@
         <v>277</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7391,10 +7391,10 @@
         <v>53</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7405,7 +7405,7 @@
         <v>278</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>